<commit_message>
finished analysis of irrigation impact. coding part done from my side
</commit_message>
<xml_diff>
--- a/data/irrigation/irrigation_main.xlsx
+++ b/data/irrigation/irrigation_main.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/ETH/code/cciwr/data/irrigation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76612117-D0B9-A047-A458-BB686B60E560}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3566B62-4863-C34D-A730-19D3D058004D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3660" yWindow="-21600" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{F5263EFD-E13A-114A-926B-CA9CAC78BE47}"/>
+    <workbookView xWindow="-4080" yWindow="-21600" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{F5263EFD-E13A-114A-926B-CA9CAC78BE47}"/>
   </bookViews>
   <sheets>
     <sheet name="AEI national" sheetId="4" r:id="rId1"/>
     <sheet name="IWU national" sheetId="3" r:id="rId2"/>
     <sheet name="AEI regional" sheetId="2" r:id="rId3"/>
     <sheet name="Crop Calendars" sheetId="5" r:id="rId4"/>
+    <sheet name="irrigation_requirement" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'AEI regional'!$1:$2</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="136">
   <si>
     <t>index</t>
   </si>
@@ -397,16 +398,68 @@
   </si>
   <si>
     <t>http://www.fao.org/nr/water/aquastat/water_use_agr/IrrigationWaterUse.pdf</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>Source: Phillips Report Appendix A page 2</t>
+  </si>
+  <si>
+    <t>irrigation_requirement</t>
+  </si>
+  <si>
+    <t>"Kolars and Mitchell states that after taking into acount potential evapotranspiration with losses that is amount withdrawn (2.5 times PE) and the return flow (35% of the amount withdrawn) the irrigation requirement becomes approximately 1.6 m (1*2.5 -(2.5*0.35)=1.6). Asuming the same distribution for the Tigris Basin with corrected consumptive use:" irrigation requirement unit is meters/month</t>
+  </si>
+  <si>
+    <t>irrigated_area_ha</t>
+  </si>
+  <si>
+    <t>irrigated_area_m2</t>
+  </si>
+  <si>
+    <t>ha2squaremeters</t>
+  </si>
+  <si>
+    <t>diversion_upstream_existing</t>
+  </si>
+  <si>
+    <t>diversion_upstream_planned</t>
+  </si>
+  <si>
+    <t>of all the planned and existing irrigation projects up- and downstream of Ilisu dam</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>m/month</t>
+  </si>
+  <si>
+    <t>diversion_downstream_planned</t>
+  </si>
+  <si>
+    <t>diversion_sum</t>
+  </si>
+  <si>
+    <t>diversion_upstream_total</t>
+  </si>
+  <si>
+    <t>seconds_per_month</t>
+  </si>
+  <si>
+    <t>m^3/s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="###\ ###\ ###\ ##0"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -451,6 +504,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="ArialMT"/>
     </font>
   </fonts>
   <fills count="2">
@@ -515,7 +573,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -549,6 +607,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -570,6 +629,7 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -2691,24 +2751,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="13.5" customHeight="1">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="20" t="s">
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="21" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A2" s="25"/>
-      <c r="B2" s="23"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="24"/>
       <c r="C2" s="11" t="s">
         <v>86</v>
       </c>
@@ -2718,7 +2778,7 @@
       <c r="E2" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="F2" s="21"/>
+      <c r="F2" s="22"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="6" t="s">
@@ -4515,8 +4575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A78E96B0-42F0-1543-ABF1-5763666B8AE4}">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4727,4 +4787,454 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F5AB7D8-9032-3448-B44A-A65C46E8107D}">
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="24.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="4" max="4" width="28.83203125" customWidth="1"/>
+    <col min="5" max="5" width="29.83203125" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="19"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="B4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5">
+        <v>121000</v>
+      </c>
+      <c r="C5">
+        <f>B5*$F$4</f>
+        <v>1210000000</v>
+      </c>
+      <c r="E5" t="s">
+        <v>134</v>
+      </c>
+      <c r="F5">
+        <f>60*60*24*31</f>
+        <v>2678400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B6">
+        <v>138000</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:C7" si="0">B6*$F$4</f>
+        <v>1380000000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7">
+        <v>375000</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>3750000000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8">
+        <f>SUM(B6:B7)</f>
+        <v>513000</v>
+      </c>
+      <c r="C8">
+        <f>SUM(C6:C7)</f>
+        <v>5130000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B9">
+        <f>SUM(B5,B8)</f>
+        <v>634000</v>
+      </c>
+      <c r="C9">
+        <f>SUM(C5,C8)</f>
+        <v>6340000000</v>
+      </c>
+      <c r="D9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13" t="s">
+        <v>135</v>
+      </c>
+      <c r="D13" t="s">
+        <v>135</v>
+      </c>
+      <c r="E13" t="s">
+        <v>135</v>
+      </c>
+      <c r="F13" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>119</v>
+      </c>
+      <c r="B14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C14" t="s">
+        <v>126</v>
+      </c>
+      <c r="D14" t="s">
+        <v>127</v>
+      </c>
+      <c r="E14" t="s">
+        <v>131</v>
+      </c>
+      <c r="F14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" s="27">
+        <v>0</v>
+      </c>
+      <c r="C15" s="27">
+        <f>B15*$C$6/$F$5</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="27">
+        <f>B15*$C$7/$F$5</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="27">
+        <f>B15*$C$5/$F$5</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="27">
+        <f>SUM(C15:E15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" s="27">
+        <v>0</v>
+      </c>
+      <c r="C16" s="27">
+        <f t="shared" ref="C16:C26" si="1">B16*$C$6/$F$5</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="27">
+        <f t="shared" ref="D16:D26" si="2">B16*$C$7/$F$5</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="27">
+        <f t="shared" ref="E16:E26" si="3">B16*$C$5/$F$5</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="27">
+        <f>SUM(C16:E16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17" s="27">
+        <v>0</v>
+      </c>
+      <c r="C17" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D17" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F17" s="27">
+        <f>SUM(C17:E17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18" s="27">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="C18" s="27">
+        <f t="shared" si="1"/>
+        <v>34.005376344086024</v>
+      </c>
+      <c r="D18" s="27">
+        <f t="shared" si="2"/>
+        <v>92.405913978494624</v>
+      </c>
+      <c r="E18" s="27">
+        <f t="shared" si="3"/>
+        <v>29.816308243727597</v>
+      </c>
+      <c r="F18" s="27">
+        <f>SUM(C18:E18)</f>
+        <v>156.22759856630825</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19" s="27">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="C19" s="27">
+        <f t="shared" si="1"/>
+        <v>68.525985663082437</v>
+      </c>
+      <c r="D19" s="27">
+        <f t="shared" si="2"/>
+        <v>186.21191756272401</v>
+      </c>
+      <c r="E19" s="27">
+        <f t="shared" si="3"/>
+        <v>60.084378733572279</v>
+      </c>
+      <c r="F19" s="27">
+        <f>SUM(C19:E19)</f>
+        <v>314.82228195937876</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <v>6</v>
+      </c>
+      <c r="B20" s="27">
+        <v>0.33400000000000002</v>
+      </c>
+      <c r="C20" s="27">
+        <f t="shared" si="1"/>
+        <v>172.08781362007167</v>
+      </c>
+      <c r="D20" s="27">
+        <f t="shared" si="2"/>
+        <v>467.6299283154122</v>
+      </c>
+      <c r="E20" s="27">
+        <f t="shared" si="3"/>
+        <v>150.88859020310633</v>
+      </c>
+      <c r="F20" s="27">
+        <f>SUM(C20:E20)</f>
+        <v>790.60633213859023</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21">
+        <v>7</v>
+      </c>
+      <c r="B21" s="27">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="C21" s="27">
+        <f t="shared" si="1"/>
+        <v>238.03763440860214</v>
+      </c>
+      <c r="D21" s="27">
+        <f t="shared" si="2"/>
+        <v>646.8413978494624</v>
+      </c>
+      <c r="E21" s="27">
+        <f t="shared" si="3"/>
+        <v>208.7141577060932</v>
+      </c>
+      <c r="F21" s="27">
+        <f>SUM(C21:E21)</f>
+        <v>1093.5931899641578</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22">
+        <v>8</v>
+      </c>
+      <c r="B22" s="27">
+        <v>0.39</v>
+      </c>
+      <c r="C22" s="27">
+        <f t="shared" si="1"/>
+        <v>200.94086021505376</v>
+      </c>
+      <c r="D22" s="27">
+        <f t="shared" si="2"/>
+        <v>546.03494623655911</v>
+      </c>
+      <c r="E22" s="27">
+        <f t="shared" si="3"/>
+        <v>176.18727598566309</v>
+      </c>
+      <c r="F22" s="27">
+        <f>SUM(C22:E22)</f>
+        <v>923.16308243727599</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23">
+        <v>9</v>
+      </c>
+      <c r="B23" s="27">
+        <v>0.187</v>
+      </c>
+      <c r="C23" s="27">
+        <f t="shared" si="1"/>
+        <v>96.348566308243733</v>
+      </c>
+      <c r="D23" s="27">
+        <f t="shared" si="2"/>
+        <v>261.81675627240145</v>
+      </c>
+      <c r="E23" s="27">
+        <f t="shared" si="3"/>
+        <v>84.479540023894856</v>
+      </c>
+      <c r="F23" s="27">
+        <f>SUM(C23:E23)</f>
+        <v>442.64486260454004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24">
+        <v>10</v>
+      </c>
+      <c r="B24" s="27">
+        <v>2.7E-2</v>
+      </c>
+      <c r="C24" s="27">
+        <f t="shared" si="1"/>
+        <v>13.911290322580646</v>
+      </c>
+      <c r="D24" s="27">
+        <f t="shared" si="2"/>
+        <v>37.802419354838712</v>
+      </c>
+      <c r="E24" s="27">
+        <f t="shared" si="3"/>
+        <v>12.19758064516129</v>
+      </c>
+      <c r="F24" s="27">
+        <f>SUM(C24:E24)</f>
+        <v>63.911290322580648</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25">
+        <v>11</v>
+      </c>
+      <c r="B25" s="27">
+        <v>0</v>
+      </c>
+      <c r="C25" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D25" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E25" s="27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F25" s="27">
+        <f>SUM(C25:E25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26">
+        <v>12</v>
+      </c>
+      <c r="B26" s="27">
+        <v>0</v>
+      </c>
+      <c r="C26" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D26" s="27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E26" s="27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="27">
+        <f>SUM(C26:E26)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>